<commit_message>
Sequence and firmware updated
</commit_message>
<xml_diff>
--- a/docs/symbol_codes.xlsx
+++ b/docs/symbol_codes.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\ouija\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C40A57F-5FBD-4D5D-8BC1-C80CED44AA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C9C58-C948-4659-83C5-E27FF54E6357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1344" yWindow="-108" windowWidth="21804" windowHeight="13176" xr2:uid="{2F8FE052-EC4B-421C-A965-19CA5C36DA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Код</t>
   </si>
@@ -144,13 +133,16 @@
   </si>
   <si>
     <t>Я</t>
+  </si>
+  <si>
+    <t>Й</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,17 +523,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23608805-7BB8-4881-B1AE-C1BAB1BFFDF1}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="8.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="8.8984375" style="2"/>
+    <col min="2" max="2" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,379 +541,382 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="2">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="2">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="2">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="2">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="2">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="2">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="2">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="2">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="2">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1">
       <c r="A49" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50" s="2">
         <v>48</v>
       </c>

</xml_diff>